<commit_message>
Add Rack in filter export
</commit_message>
<xml_diff>
--- a/Received Report.xlsx
+++ b/Received Report.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
-  <si>
-    <t>CENTRAL NEGROS POWER RELIABILITY, INC.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+  <si>
+    <t>PROGEN DIESEL TECH</t>
   </si>
   <si>
     <t>Purok San Jose, Brgy. Calumangan, Bago City</t>
@@ -35,13 +35,13 @@
     <t>TO</t>
   </si>
   <si>
-    <t>2019-02-01</t>
+    <t>2019-06-01</t>
   </si>
   <si>
     <t>FROM</t>
   </si>
   <si>
-    <t>2019-03-28</t>
+    <t>2019-08-06</t>
   </si>
   <si>
     <t>Warehouse</t>
@@ -89,29 +89,173 @@
     <t>End Use</t>
   </si>
   <si>
-    <t>2019-03-20</t>
+    <t>2019-07-01</t>
+  </si>
+  <si>
+    <t>PROR-162-2019</t>
+  </si>
+  <si>
+    <t>CON-CON_1002</t>
+  </si>
+  <si>
+    <t>Paint Brush 1"</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Greenlane Hardware and Construction Supply Inc</t>
+  </si>
+  <si>
+    <t>Progen Warehouse</t>
+  </si>
+  <si>
+    <t>Consumables / Cleaning &amp; Preservation of Spare parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progen Warehouse
+</t>
+  </si>
+  <si>
+    <t>2019-06-29</t>
+  </si>
+  <si>
+    <t>PROR-234-2019</t>
+  </si>
+  <si>
+    <t>CON-FUE_1001</t>
+  </si>
+  <si>
+    <t>Diesel, Fuel-Save</t>
+  </si>
+  <si>
+    <t>ltr/s</t>
+  </si>
+  <si>
+    <t>Sum-ag Petron Gas Station</t>
+  </si>
+  <si>
+    <t>Progen CV</t>
+  </si>
+  <si>
+    <t>Dismantling, cleaning, inspection, crack testing, measurement &amp; evaluation, reassembling &amp; preservation.</t>
+  </si>
+  <si>
+    <t>DG4 (CV Area) Main Engine Parts &amp; Components</t>
+  </si>
+  <si>
+    <t>2019-06-28</t>
+  </si>
+  <si>
+    <t>PROR-131-2019</t>
+  </si>
+  <si>
+    <t>BUI-MAT_1001</t>
+  </si>
+  <si>
+    <t>Plywood, Ordinary, 4.5mm x 8ft</t>
+  </si>
+  <si>
+    <t>sht/s</t>
+  </si>
+  <si>
+    <t>A-one Industrial Hardware</t>
+  </si>
+  <si>
+    <t>Fabrication of Wooden Crates for DG1 Engine Parts (Pistons &amp; Connecting Rods)</t>
+  </si>
+  <si>
+    <t>DG1 (CV Area) Main Engine Parts &amp; Components.</t>
+  </si>
+  <si>
+    <t>CON-CHE_1001</t>
+  </si>
+  <si>
+    <t>Vappro 868 VCI Corrosion Inbitor Wax Coating (4 liters/gallon)</t>
+  </si>
+  <si>
+    <t>gal/s</t>
+  </si>
+  <si>
+    <t>Impact One Nation Industrial Corporation</t>
+  </si>
+  <si>
+    <t>PROR-173-2019</t>
+  </si>
+  <si>
+    <t>2019-06-22</t>
   </si>
   <si>
     <t>begbal</t>
   </si>
   <si>
-    <t>005Q022</t>
-  </si>
-  <si>
-    <t>Oil Scrapper PF 5-22</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accounting Department
-</t>
-  </si>
-  <si>
-    <t>40MVA Power Transformer Secondary Bus Framing/Support</t>
-  </si>
-  <si>
-    <t>1.5 MVA Station Transformer DG4 &amp; DG5 Generator Winding/VCB/MOCB/Cable Monitor</t>
+    <t>PRO-PF 32-249A</t>
+  </si>
+  <si>
+    <t>Spring Guide</t>
+  </si>
+  <si>
+    <t>Progen</t>
+  </si>
+  <si>
+    <t>Inventory Beginning Balance</t>
+  </si>
+  <si>
+    <t>Warehouse Beginning Balance</t>
+  </si>
+  <si>
+    <t>2019-06-20</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>_1001</t>
+  </si>
+  <si>
+    <t>O-ring, 10mm ID x 14mm OD x 2mmT</t>
+  </si>
+  <si>
+    <t>7RJ Brothers Sand &amp; Gravel &amp; Gen. Mdse.</t>
+  </si>
+  <si>
+    <t>Bacolod HR</t>
+  </si>
+  <si>
+    <t>Additional Padlock for Reconditioning Equipment Tool Cabinet</t>
+  </si>
+  <si>
+    <t>40 MVA Power Transformer</t>
+  </si>
+  <si>
+    <t>2019-06-10</t>
+  </si>
+  <si>
+    <t>MTG Gasoline Service Station</t>
+  </si>
+  <si>
+    <t>2019-06-04</t>
+  </si>
+  <si>
+    <t>CON-FUE_1002</t>
+  </si>
+  <si>
+    <t>Penetrating Oil Multi Use, WD40</t>
+  </si>
+  <si>
+    <t>can/s</t>
+  </si>
+  <si>
+    <t>C.Y. Ong Multi-Distributor</t>
+  </si>
+  <si>
+    <t>2019-06-03</t>
+  </si>
+  <si>
+    <t>CON-CON_1001</t>
+  </si>
+  <si>
+    <t>Scraper, Industrial; Size: 2"</t>
   </si>
   <si>
     <t xml:space="preserve">Prepared By: </t>
@@ -632,7 +776,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="N2" sqref="N2"/>
@@ -849,88 +993,598 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="2">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="2">
+        <v>21</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="3">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2">
+        <v>10</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" t="s">
+      <c r="A14" s="3">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="2">
+        <v>3</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="3">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="2">
+        <v>6</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="3">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2">
+        <v>32</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17" s="3">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="2">
+        <v>10</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" s="3">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:26">
-      <c r="A17" t="s">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D17" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="2">
+        <v>19</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19" s="3">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="2">
+        <v>18</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20" s="3">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="2">
+        <v>6</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21" s="3">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="2">
+        <v>10</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
     <protectedRange name="p1aa278975760d5a8789fe736a4242e4f" sqref="A11:Z11" password="C724"/>
-    <protectedRange name="pb92778bd78a4353a4ab9294156805e41" sqref="A14:AC14" password="C724"/>
-    <protectedRange name="p3a834472df22454fed33e8b780f2ec25" sqref="A16:AC16" password="C724"/>
+    <protectedRange name="p2d50bcfbfb59eed8c1608c98599dde33" sqref="A12:Z12" password="C724"/>
+    <protectedRange name="pc1a4c45411a7b95306d8a232689e20b1" sqref="A13:Z13" password="C724"/>
+    <protectedRange name="p8719be3b033d56416c2459d20ed7acf0" sqref="A14:Z14" password="C724"/>
+    <protectedRange name="p430addb3dd5b129a90e87b2af7db32cf" sqref="A15:Z15" password="C724"/>
+    <protectedRange name="pdac316cf8e611047934990c6afb0100a" sqref="A16:Z16" password="C724"/>
+    <protectedRange name="pac6911475955aba68a711565feae3a6a" sqref="A17:Z17" password="C724"/>
+    <protectedRange name="pcc518def6f8a4eb777dc6a8a1cb23e74" sqref="A18:Z18" password="C724"/>
+    <protectedRange name="p7a00206c9f8849998c8649eff43c8cd5" sqref="A19:Z19" password="C724"/>
+    <protectedRange name="p00866f9227b5920e8af5a41faf505954" sqref="A20:Z20" password="C724"/>
+    <protectedRange name="pb5d212ac1780894358016b591d961e29" sqref="A21:Z21" password="C724"/>
+    <protectedRange name="p1627ec246080e388511f0e2e333f62b2" sqref="A24:AC24" password="C724"/>
+    <protectedRange name="p9f36a12064855111794ae27561c69276" sqref="A26:AC26" password="C724"/>
   </protectedRanges>
   <mergeCells>
     <mergeCell ref="B12:C12"/>
@@ -950,6 +1604,96 @@
     <mergeCell ref="U12:W12"/>
     <mergeCell ref="X11:Z11"/>
     <mergeCell ref="X12:Z12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="X13:Z13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="X16:Z16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="X17:Z17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="X18:Z18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="X19:Z19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="X20:Z20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="X21:Z21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="X22:Z22"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>

</xml_diff>

<commit_message>
fixed export displaying of mrwf no and mif no in inventory report
</commit_message>
<xml_diff>
--- a/Received Report.xlsx
+++ b/Received Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
   <si>
     <t>PROGEN Dieseltech Services Corp.</t>
   </si>
@@ -38,13 +38,13 @@
     <t>FROM</t>
   </si>
   <si>
-    <t>2021-04-02</t>
+    <t>2021-05-01</t>
   </si>
   <si>
     <t>TO</t>
   </si>
   <si>
-    <t>2021-07-05</t>
+    <t>2021-05-31</t>
   </si>
   <si>
     <t>Warehouse</t>
@@ -107,139 +107,343 @@
     <t>End Use</t>
   </si>
   <si>
-    <t>2021-06-11</t>
-  </si>
-  <si>
-    <t>sample100</t>
-  </si>
-  <si>
-    <t>MRIF-2021-06-0019</t>
-  </si>
-  <si>
-    <t>sample1001</t>
-  </si>
-  <si>
-    <t>AUX-PAR_1294</t>
-  </si>
-  <si>
-    <t>Key, SJ6-G9</t>
+    <t>2021-05-29</t>
+  </si>
+  <si>
+    <t>PIPRO21-1137-1655-PRGN</t>
+  </si>
+  <si>
+    <t>1652-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0292</t>
+  </si>
+  <si>
+    <t>IPRO21-1137-PRGN / PROPR-BCD21-106</t>
+  </si>
+  <si>
+    <t>CON-CHE_1017</t>
+  </si>
+  <si>
+    <t>Gasoline, Unleaded</t>
+  </si>
+  <si>
+    <t>ltr/s</t>
+  </si>
+  <si>
+    <t>Sum-ag Petron Gas Station</t>
+  </si>
+  <si>
+    <t>ECMG</t>
+  </si>
+  <si>
+    <t>Consumables of Cleaning and Clearing</t>
+  </si>
+  <si>
+    <t>Progen Spare Parts</t>
+  </si>
+  <si>
+    <t>PWHP21-1136-1653-PRGN</t>
+  </si>
+  <si>
+    <t>1650-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0291</t>
+  </si>
+  <si>
+    <t>WHP21-1136-PRGN / PROPR-BCD21-105</t>
+  </si>
+  <si>
+    <t>CON-FUE_1001</t>
+  </si>
+  <si>
+    <t>Diesel, Fuel-Save</t>
+  </si>
+  <si>
+    <t>Progen Warehouse</t>
+  </si>
+  <si>
+    <t>Refuel for Heavy Equipment</t>
+  </si>
+  <si>
+    <t>Heavy Equipment - Forklift</t>
+  </si>
+  <si>
+    <t>2021-05-20</t>
+  </si>
+  <si>
+    <t>PIPRO21-1135-1652-PRGN</t>
+  </si>
+  <si>
+    <t>1649-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0290</t>
+  </si>
+  <si>
+    <t>IPRO21-1135-PRGN / PROPR-BCD21-104</t>
+  </si>
+  <si>
+    <t>CON-CON_1060</t>
+  </si>
+  <si>
+    <t>Thinner, Acrylic</t>
+  </si>
+  <si>
+    <t>gal/s</t>
+  </si>
+  <si>
+    <t>Bacolod Luis Paint Center Enterprises</t>
+  </si>
+  <si>
+    <t>Consumables for Reconditioning and Painting</t>
+  </si>
+  <si>
+    <t>DG1 (CV Area) Main Engine Parts &amp; Components.</t>
+  </si>
+  <si>
+    <t>PIPRO21-1134-1651-PRGN</t>
+  </si>
+  <si>
+    <t>1648-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0289</t>
+  </si>
+  <si>
+    <t>IPRO21-1134-PRGN / PROPR-BCD21-103</t>
+  </si>
+  <si>
+    <t>Progen CV Area</t>
+  </si>
+  <si>
+    <t>PIPRO21-1134-1650-PRGN</t>
+  </si>
+  <si>
+    <t>1647-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0288</t>
+  </si>
+  <si>
+    <t>PIPRO21-1134-1649-PRGN</t>
+  </si>
+  <si>
+    <t>1646-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0287</t>
+  </si>
+  <si>
+    <t>CON-HOU_1003</t>
+  </si>
+  <si>
+    <t>Gloves, Cotton</t>
+  </si>
+  <si>
+    <t>pair/s</t>
+  </si>
+  <si>
+    <t>Greenlane Hardware and Construction Supply Inc</t>
+  </si>
+  <si>
+    <t>2021-05-17</t>
+  </si>
+  <si>
+    <t>POPE21-1039-1056-PRGN-MNL-R1</t>
+  </si>
+  <si>
+    <t>DR-PROGENMNL-005</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0286</t>
+  </si>
+  <si>
+    <t>OPE21-1039-PRGN-MNL / PROPR-BCD21-030</t>
+  </si>
+  <si>
+    <t>CON-CHE_1006</t>
+  </si>
+  <si>
+    <t>Crack Detector, Cleaner, Spotcheck, SKC-S Aerosol</t>
+  </si>
+  <si>
+    <t>can/s</t>
+  </si>
+  <si>
+    <t>Cifra Marketing Corporation</t>
+  </si>
+  <si>
+    <t>Additional Consumables for Refurbishing/Reconditioning</t>
+  </si>
+  <si>
+    <t>18 Units Valve Gear Assembly</t>
+  </si>
+  <si>
+    <t>CON-CHE_1007</t>
+  </si>
+  <si>
+    <t>Crack Detector, Developer, Spotcheck, SKD-S2</t>
+  </si>
+  <si>
+    <t>CON-CHE_1008</t>
+  </si>
+  <si>
+    <t>Crack Detector, Penetrant, Spotcheck, SKL-SP2</t>
+  </si>
+  <si>
+    <t>PWHP21-1032-1049-PRGN-MNL-R1</t>
+  </si>
+  <si>
+    <t>DR-PROGENMNL-004</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0285</t>
+  </si>
+  <si>
+    <t>WHP21-1032-PRGN-MNL / PROGEN-071-2020</t>
+  </si>
+  <si>
+    <t>Consumables for Refurbishing  / Reconditioning</t>
+  </si>
+  <si>
+    <t>Refurbishing of 36 units Cylinder Liner with Water Jacket</t>
+  </si>
+  <si>
+    <t>2021-05-15</t>
+  </si>
+  <si>
+    <t>PIPRO21-1133-1648-PRGN</t>
+  </si>
+  <si>
+    <t>1645-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0284</t>
+  </si>
+  <si>
+    <t>IPRO21-1133-PRGN / PROPR-BCD21-091</t>
+  </si>
+  <si>
+    <t>CON-EIC_1003</t>
+  </si>
+  <si>
+    <t>Battery, AAA</t>
   </si>
   <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>A.C. Parts Merchandising</t>
-  </si>
-  <si>
-    <t>Bacolod HR</t>
-  </si>
-  <si>
-    <t>Auto Start/Stop of Deep Well Pump Refill to Raw Water Tank</t>
-  </si>
-  <si>
-    <t>4 Units Cylinder Head (Bare) for CPGC</t>
-  </si>
-  <si>
-    <t>2021-06-09</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>MRIF-2021-06-0018</t>
-  </si>
-  <si>
-    <t>Test sAmple</t>
-  </si>
-  <si>
-    <t>K 47224</t>
-  </si>
-  <si>
-    <t>3-way Valve, Complete</t>
-  </si>
-  <si>
-    <t>2GO Express</t>
-  </si>
-  <si>
-    <t>ECMG</t>
-  </si>
-  <si>
-    <t>Progen Consumables</t>
-  </si>
-  <si>
-    <t>DG2 Main Engine Frame Cleaning and Preserving</t>
-  </si>
-  <si>
-    <t>2021-05-12</t>
-  </si>
-  <si>
-    <t>MRIF-2021-05-0017</t>
-  </si>
-  <si>
-    <t>sample-2001-2021</t>
-  </si>
-  <si>
-    <t>A-1 Gas Corporation</t>
-  </si>
-  <si>
-    <t>Environment/PCO</t>
-  </si>
-  <si>
-    <t>Additional Padlock for Reconditioning Equipment Tool Cabinet</t>
-  </si>
-  <si>
-    <t>125 Vdc Battery Charger</t>
-  </si>
-  <si>
-    <t>sample-1050-20212</t>
-  </si>
-  <si>
-    <t>sample-1050-20211</t>
-  </si>
-  <si>
-    <t>MRIF-2021-05-0016</t>
-  </si>
-  <si>
-    <t>sample-1001-2021</t>
-  </si>
-  <si>
-    <t>K 27046 B</t>
-  </si>
-  <si>
-    <t>(BIG) Tubular Sealing for Cover K 27007 and Bearing Casing K 28001</t>
-  </si>
-  <si>
-    <t>7-Eleven, LLARC Convenience Store</t>
-  </si>
-  <si>
-    <t>Additional Sludge Recovery Storage</t>
-  </si>
-  <si>
-    <t>12 Units Connecting Rod Assembly and 12 Units Piston Assembly</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>MRIF-2021-05-0015</t>
-  </si>
-  <si>
-    <t>K 47034</t>
+    <t>SM Supermarket</t>
+  </si>
+  <si>
+    <t>Replacement of Drained Battery</t>
+  </si>
+  <si>
+    <t>Thickness Gauge</t>
+  </si>
+  <si>
+    <t>PWHP21-1131-1638-PRGN</t>
+  </si>
+  <si>
+    <t>1635-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0283</t>
+  </si>
+  <si>
+    <t>WHP21-1131-PRGN / PROPR-BCD21-090</t>
+  </si>
+  <si>
+    <t>FFE-OFF_1005</t>
+  </si>
+  <si>
+    <t>Padlock; long shackle, 40mm</t>
+  </si>
+  <si>
+    <t>Ace Hardware Philippines, Inc. - Bacolod Branch</t>
+  </si>
+  <si>
+    <t>Replacement of Damaged Padlock</t>
+  </si>
+  <si>
+    <t>Container Vans</t>
   </si>
   <si>
     <t>2021-05-10</t>
   </si>
   <si>
-    <t>MRIF-2021-05-0014</t>
-  </si>
-  <si>
-    <t>ECMG20-1021</t>
-  </si>
-  <si>
-    <t>Equipment for Engine Parts Thickness Gauge Measurement</t>
-  </si>
-  <si>
-    <t>Engine Parts</t>
+    <t>PIPRO21-1124-1585-PRGN</t>
+  </si>
+  <si>
+    <t>1583-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0282</t>
+  </si>
+  <si>
+    <t>IPRO21-1124-PRGN / PROPR-BCD21-068</t>
+  </si>
+  <si>
+    <t>CON-CHE_1011</t>
+  </si>
+  <si>
+    <t>Acetylene</t>
+  </si>
+  <si>
+    <t>cyl/s</t>
+  </si>
+  <si>
+    <t>Bacolod Oxygen Acetylene Gas Corp.</t>
+  </si>
+  <si>
+    <t>Fabrication</t>
+  </si>
+  <si>
+    <t>Transition Piece Bracket</t>
+  </si>
+  <si>
+    <t>PIPRO21-1124-1584-PRGN</t>
+  </si>
+  <si>
+    <t>1582-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0281</t>
+  </si>
+  <si>
+    <t>CON-CHE_1010</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>2021-05-06</t>
+  </si>
+  <si>
+    <t>PWHP21-1079-1552-PRGN</t>
+  </si>
+  <si>
+    <t>1550-PRGN</t>
+  </si>
+  <si>
+    <t>MRIF-2021-05-0280</t>
+  </si>
+  <si>
+    <t>WHP21-1079 / PROGEN-071-2020</t>
+  </si>
+  <si>
+    <t>CON-HOU_1001</t>
+  </si>
+  <si>
+    <t>Rags, Cotton</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>Procolors T-Shirts Printing</t>
   </si>
   <si>
     <t xml:space="preserve">Prepared By: </t>
@@ -763,7 +967,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="N2" sqref="N2"/>
@@ -1034,55 +1238,55 @@
         <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="2">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R11" s="2">
-        <v>1001</v>
+        <v>51.1</v>
       </c>
       <c r="S11" s="2">
-        <v>100100</v>
+        <v>1533</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AD11" s="1"/>
       <c r="AE11" s="1"/>
@@ -1092,45 +1296,47 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="2">
-        <v>23</v>
-      </c>
-      <c r="Q12" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="R12" s="2">
-        <v>2344</v>
+        <v>40.3</v>
       </c>
       <c r="S12" s="2">
-        <v>53912</v>
+        <v>1612</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
@@ -1158,57 +1364,59 @@
         <v>51</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="1">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1">
-        <v>12</v>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="2">
-        <v>100</v>
-      </c>
-      <c r="Q13" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="R13" s="2">
-        <v>1101</v>
+        <v>400</v>
       </c>
       <c r="S13" s="2">
-        <v>110100</v>
+        <v>400</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
@@ -1222,51 +1430,53 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="2">
-        <v>200</v>
-      </c>
-      <c r="Q14" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="R14" s="2">
-        <v>110</v>
+        <v>50.4</v>
       </c>
       <c r="S14" s="2">
-        <v>22000</v>
+        <v>957.6</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
@@ -1288,48 +1498,50 @@
         <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="2">
-        <v>50</v>
-      </c>
-      <c r="Q15" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="R15" s="2">
-        <v>1001</v>
+        <v>50.4</v>
       </c>
       <c r="S15" s="2">
-        <v>50050</v>
+        <v>554.4</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
@@ -1344,110 +1556,701 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="R16" s="2">
-        <v>100</v>
+        <v>11.45</v>
       </c>
       <c r="S16" s="2">
-        <v>1000</v>
+        <v>229</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
     </row>
     <row r="17" spans="1:31">
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-      <c r="N17"/>
-      <c r="O17"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17"/>
-      <c r="U17"/>
-      <c r="V17"/>
-      <c r="W17"/>
-      <c r="X17"/>
-      <c r="Y17"/>
-      <c r="Z17"/>
-      <c r="AA17"/>
-      <c r="AB17"/>
-      <c r="AC17"/>
-      <c r="AD17"/>
-      <c r="AE17"/>
+      <c r="A17" s="1">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R17" s="2">
+        <v>880</v>
+      </c>
+      <c r="S17" s="2">
+        <v>5280</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+    </row>
+    <row r="18" spans="1:31">
+      <c r="A18" s="1">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R18" s="2">
+        <v>750</v>
+      </c>
+      <c r="S18" s="2">
+        <v>2250</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
     </row>
     <row r="19" spans="1:31">
-      <c r="A19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="A19" s="1">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R19" s="2">
+        <v>750</v>
+      </c>
+      <c r="S19" s="2">
+        <v>2250</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+    </row>
+    <row r="20" spans="1:31">
+      <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R20" s="2">
+        <v>880</v>
+      </c>
+      <c r="S20" s="2">
+        <v>10560</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+    </row>
+    <row r="21" spans="1:31">
+      <c r="A21" s="1">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R21" s="2">
+        <v>24.25</v>
+      </c>
+      <c r="S21" s="2">
+        <v>97</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" t="s">
-        <v>80</v>
+      <c r="A22" s="1">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R22" s="2">
+        <v>299.75</v>
+      </c>
+      <c r="S22" s="2">
+        <v>3597</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+    </row>
+    <row r="23" spans="1:31">
+      <c r="A23" s="1">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1100</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1100</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+    </row>
+    <row r="24" spans="1:31">
+      <c r="A24" s="1">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="R24" s="2">
+        <v>400</v>
+      </c>
+      <c r="S24" s="2">
+        <v>800</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+    </row>
+    <row r="25" spans="1:31">
+      <c r="A25" s="1">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="R25" s="2">
+        <v>50</v>
+      </c>
+      <c r="S25" s="2">
+        <v>750</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+    </row>
+    <row r="26" spans="1:31">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+      <c r="Z26"/>
+      <c r="AA26"/>
+      <c r="AB26"/>
+      <c r="AC26"/>
+      <c r="AD26"/>
+      <c r="AE26"/>
+    </row>
+    <row r="28" spans="1:31">
+      <c r="A28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1459,8 +2262,17 @@
     <protectedRange name="ped1d181546acc2399661c6c40a9beb6a" sqref="A14:AE14" password="C724"/>
     <protectedRange name="p0bef65a3b969817700b25eca80231809" sqref="A15:AE15" password="C724"/>
     <protectedRange name="p3c3ae308d44e1437db7fec4ac824dcbe" sqref="A16:AE16" password="C724"/>
-    <protectedRange name="pcb0e4452152caf01f2ddcab59aa774ed" sqref="A19:AC19" password="C724"/>
-    <protectedRange name="p19f680c13282bb793df96480af2f729d" sqref="A21:AC21" password="C724"/>
+    <protectedRange name="pbaf01c4f8129bac3b495ed6ce3d7a20d" sqref="A17:AE17" password="C724"/>
+    <protectedRange name="p1ed67d8fdcda9026ac46d214b4bd359f" sqref="A18:AE18" password="C724"/>
+    <protectedRange name="p91aa4b373289228480b772312167e8b1" sqref="A19:AE19" password="C724"/>
+    <protectedRange name="p79578f6982ac118ac396f49115536361" sqref="A20:AE20" password="C724"/>
+    <protectedRange name="p04e5167e000f3412892a0a6d88eaa380" sqref="A21:AE21" password="C724"/>
+    <protectedRange name="pa92ae8861d22f65476c5fc157c499054" sqref="A22:AE22" password="C724"/>
+    <protectedRange name="pd710f6020a662be45f43bbebee1a0a85" sqref="A23:AE23" password="C724"/>
+    <protectedRange name="p3002bf9e6fdaae719a4a5fd015a50ca4" sqref="A24:AE24" password="C724"/>
+    <protectedRange name="p8dfa80e9f3d51a22d980a49bae761b35" sqref="A25:AE25" password="C724"/>
+    <protectedRange name="p807bd27742240b7001ab7b50e6be40d4" sqref="A28:AC28" password="C724"/>
+    <protectedRange name="pfcf687de1ec7fbd2e3ac88905f396410" sqref="A30:AC30" password="C724"/>
   </protectedRanges>
   <mergeCells>
     <mergeCell ref="B12:C12"/>
@@ -1525,6 +2337,87 @@
     <mergeCell ref="X17:Y17"/>
     <mergeCell ref="Z17:AB17"/>
     <mergeCell ref="AC17:AE17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="T19:W19"/>
+    <mergeCell ref="X19:Y19"/>
+    <mergeCell ref="Z19:AB19"/>
+    <mergeCell ref="AC19:AE19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="T20:W20"/>
+    <mergeCell ref="X20:Y20"/>
+    <mergeCell ref="Z20:AB20"/>
+    <mergeCell ref="AC20:AE20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="T21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AB21"/>
+    <mergeCell ref="AC21:AE21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="T22:W22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AB22"/>
+    <mergeCell ref="AC22:AE22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="T23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AB23"/>
+    <mergeCell ref="AC23:AE23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="T24:W24"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="Z24:AB24"/>
+    <mergeCell ref="AC24:AE24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="T25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="Z25:AB25"/>
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="T26:W26"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="Z26:AB26"/>
+    <mergeCell ref="AC26:AE26"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F10:G10"/>

</xml_diff>